<commit_message>
Fix flake8 errors in atomic_piston.py
</commit_message>
<xml_diff>
--- a/atomic_piston/IPU/presupuesto_ipu.xlsx
+++ b/atomic_piston/IPU/presupuesto_ipu.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardomayor/Documents/GitHub/watchers_refined/atomic_piston/IPU/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C2D27B-F2C1-C340-989F-B6293BDD9476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Genera un presupuesto con las c" sheetId="1" r:id="rId4"/>
+    <sheet name="Genera un presupuesto con las c" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -181,15 +190,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -200,11 +210,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="12">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF284E3F"/>
@@ -218,6 +234,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -232,6 +249,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -246,48 +264,52 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -302,6 +324,7 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -316,6 +339,7 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -330,147 +354,139 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6F8F9"/>
+          <bgColor rgb="FFF6F8F9"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF356854"/>
           <bgColor rgb="FF356854"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6F8F9"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Genera un presupuesto con las c-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Genera un presupuesto con las c-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D20" displayName="Tabla_1" name="Tabla_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla_1" displayName="Tabla_1" ref="A1:D20">
   <tableColumns count="4">
-    <tableColumn name="Categoría" id="1"/>
-    <tableColumn name="Componente" id="2"/>
-    <tableColumn name="Cantidad" id="3"/>
-    <tableColumn name="Notas" id="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Categoría"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Componente"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cantidad"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Notas"/>
   </tableColumns>
-  <tableStyleInfo name="Genera un presupuesto con las c-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Genera un presupuesto con las c-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -660,28 +676,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.38"/>
-    <col customWidth="1" min="2" max="2" width="37.63"/>
-    <col customWidth="1" min="4" max="4" width="37.63"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -709,7 +728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -723,7 +742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
@@ -734,7 +753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
@@ -745,7 +764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -756,7 +775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -770,7 +789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
@@ -781,7 +800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
@@ -792,7 +811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -806,7 +825,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
@@ -817,7 +836,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
@@ -828,7 +847,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
@@ -842,7 +861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
@@ -853,7 +872,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -867,7 +886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>41</v>
       </c>
@@ -878,7 +897,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="8" t="s">
         <v>44</v>
       </c>
@@ -889,7 +908,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="5" t="s">
         <v>47</v>
       </c>
@@ -900,7 +919,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="8" t="s">
         <v>50</v>
       </c>
@@ -911,7 +930,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="10" t="s">
         <v>53</v>
       </c>
@@ -923,9 +942,9 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>